<commit_message>
Adding a new indicator
</commit_message>
<xml_diff>
--- a/indicators.xlsx
+++ b/indicators.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Daymler\daymler\UNIDO\09_Project\my_new_page\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Daymler\daymler\UNIDO\09_Project\my_new_adj\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67E7CBCB-0D3B-465E-888E-BC2ABC554487}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A485F35-A012-4550-8661-B5DA76166577}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="indicators" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="222">
   <si>
     <t>Category</t>
   </si>
@@ -700,6 +700,18 @@
       </rPr>
       <t xml:space="preserve"> emissions/MVA</t>
     </r>
+  </si>
+  <si>
+    <t>Expected investment</t>
+  </si>
+  <si>
+    <t>Expected Investment reflects the anticipated financial commitment investors are willing to allocate toward industry projects.</t>
+  </si>
+  <si>
+    <t>Market research reports, investor surveys and commitments, historical data on investment trends in similar sectors</t>
+  </si>
+  <si>
+    <t>Forecasted financial return of project i  x  The probability of project being funded, based on market analysis, investor surveys, and financial feasibility</t>
   </si>
 </sst>
 </file>
@@ -1191,9 +1203,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1550,19 +1563,19 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:E65"/>
+  <dimension ref="A1:E66"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A69" sqref="A69"/>
+    <sheetView tabSelected="1" zoomScale="107" zoomScaleNormal="107" workbookViewId="0">
+      <selection activeCell="D66" sqref="D66"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.85546875" customWidth="1"/>
-    <col min="2" max="2" width="54.28515625" customWidth="1"/>
+    <col min="1" max="1" width="20.88671875" customWidth="1"/>
+    <col min="2" max="2" width="54.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1579,7 +1592,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>152</v>
       </c>
@@ -1596,7 +1609,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="3" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>152</v>
       </c>
@@ -1613,7 +1626,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="4" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>152</v>
       </c>
@@ -1630,7 +1643,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="5" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>152</v>
       </c>
@@ -1647,7 +1660,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="6" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>152</v>
       </c>
@@ -1664,7 +1677,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="7" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>152</v>
       </c>
@@ -1681,7 +1694,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="8" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -1698,7 +1711,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -1715,7 +1728,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>5</v>
       </c>
@@ -1732,7 +1745,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>5</v>
       </c>
@@ -1749,7 +1762,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="12" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>5</v>
       </c>
@@ -1766,7 +1779,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="13" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>5</v>
       </c>
@@ -1783,7 +1796,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>25</v>
       </c>
@@ -1800,7 +1813,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>30</v>
       </c>
@@ -1817,7 +1830,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="16" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>25</v>
       </c>
@@ -1834,7 +1847,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>25</v>
       </c>
@@ -1848,7 +1861,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>30</v>
       </c>
@@ -1865,7 +1878,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>30</v>
       </c>
@@ -1882,7 +1895,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="20" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>30</v>
       </c>
@@ -1899,7 +1912,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="21" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>30</v>
       </c>
@@ -1916,7 +1929,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="22" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>47</v>
       </c>
@@ -1933,7 +1946,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="23" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>47</v>
       </c>
@@ -1950,7 +1963,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="24" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>47</v>
       </c>
@@ -1967,7 +1980,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="25" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>47</v>
       </c>
@@ -1984,7 +1997,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="26" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>47</v>
       </c>
@@ -2001,7 +2014,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="27" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>47</v>
       </c>
@@ -2018,7 +2031,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="28" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>47</v>
       </c>
@@ -2035,7 +2048,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="29" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>63</v>
       </c>
@@ -2052,7 +2065,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="30" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>63</v>
       </c>
@@ -2069,7 +2082,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="31" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>63</v>
       </c>
@@ -2086,7 +2099,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="32" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>63</v>
       </c>
@@ -2103,7 +2116,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="33" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>63</v>
       </c>
@@ -2120,7 +2133,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="34" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>63</v>
       </c>
@@ -2137,7 +2150,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="35" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>63</v>
       </c>
@@ -2154,7 +2167,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="36" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>137</v>
       </c>
@@ -2171,7 +2184,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="37" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>137</v>
       </c>
@@ -2188,7 +2201,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="38" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>137</v>
       </c>
@@ -2205,7 +2218,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="39" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>137</v>
       </c>
@@ -2222,7 +2235,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="40" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>137</v>
       </c>
@@ -2239,7 +2252,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="41" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>137</v>
       </c>
@@ -2256,7 +2269,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="42" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>137</v>
       </c>
@@ -2273,7 +2286,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="43" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>96</v>
       </c>
@@ -2290,7 +2303,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="44" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>96</v>
       </c>
@@ -2307,7 +2320,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="45" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>96</v>
       </c>
@@ -2324,7 +2337,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="46" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>96</v>
       </c>
@@ -2341,7 +2354,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="47" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>25</v>
       </c>
@@ -2358,7 +2371,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="48" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>96</v>
       </c>
@@ -2375,7 +2388,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="49" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>111</v>
       </c>
@@ -2392,7 +2405,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="50" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>111</v>
       </c>
@@ -2409,7 +2422,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="51" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>111</v>
       </c>
@@ -2426,7 +2439,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="52" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>111</v>
       </c>
@@ -2443,7 +2456,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>111</v>
       </c>
@@ -2460,7 +2473,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="54" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>142</v>
       </c>
@@ -2477,7 +2490,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="55" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>142</v>
       </c>
@@ -2494,7 +2507,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="56" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>142</v>
       </c>
@@ -2511,7 +2524,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="57" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>142</v>
       </c>
@@ -2528,7 +2541,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="58" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>142</v>
       </c>
@@ -2545,7 +2558,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="59" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>142</v>
       </c>
@@ -2562,7 +2575,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="60" spans="1:5" ht="18" hidden="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:5" ht="15.6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>25</v>
       </c>
@@ -2579,7 +2592,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="61" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>141</v>
       </c>
@@ -2596,7 +2609,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="62" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>141</v>
       </c>
@@ -2613,7 +2626,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="63" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>141</v>
       </c>
@@ -2630,7 +2643,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="64" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>141</v>
       </c>
@@ -2647,7 +2660,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="65" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>141</v>
       </c>
@@ -2662,6 +2675,23 @@
       </c>
       <c r="E65" t="s">
         <v>147</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>137</v>
+      </c>
+      <c r="B66" t="s">
+        <v>218</v>
+      </c>
+      <c r="C66" t="s">
+        <v>219</v>
+      </c>
+      <c r="D66" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="E66" t="s">
+        <v>220</v>
       </c>
     </row>
   </sheetData>

</xml_diff>